<commit_message>
Tested Photoreceptor generation with correct distribution, added Excel file showing results.
</commit_message>
<xml_diff>
--- a/Retina Project Beta/Topography Data.xlsx
+++ b/Retina Project Beta/Topography Data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -2568,7 +2568,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Improved data quality and correctness
</commit_message>
<xml_diff>
--- a/Retina Project Beta/Topography Data.xlsx
+++ b/Retina Project Beta/Topography Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Eccentricity</t>
   </si>
@@ -35,7 +35,10 @@
     <t>Rods/mm2 (x1000)</t>
   </si>
   <si>
-    <t xml:space="preserve">git </t>
+    <t>Eccentricity (mm)</t>
+  </si>
+  <si>
+    <t>GC/mm2 (x1000)</t>
   </si>
 </sst>
 </file>
@@ -71,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,7 +173,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -192,90 +196,17 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.12218999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.9600897000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17.499040000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26.761690000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35.514499999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>54.506880000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>72.426950000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90.751599999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>108.60589</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>126.01612</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>144.24867</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>162.93843000000001</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>Sheet1!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>201.81899999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>150.17026999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>111.00869</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>88.492249999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>69.915450000000007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50.293564000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41.721465999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35.550727999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>30.941756999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>26.3093</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>25.686942999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>24.295444</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -684,52 +615,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>9.1478859999999997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.805035</c:v>
+                  <c:v>5.3633199999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.424519</c:v>
+                  <c:v>9.8615900000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.263339999999999</c:v>
+                  <c:v>0.147059</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.181919999999998</c:v>
+                  <c:v>0.198962</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.723860000000002</c:v>
+                  <c:v>0.30103799999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62.198535999999997</c:v>
+                  <c:v>0.39619399999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.363839999999996</c:v>
+                  <c:v>0.49826999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>79.412025</c:v>
+                  <c:v>0.59515600000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>88.886700000000005</c:v>
+                  <c:v>0.69550199999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>98.371346000000003</c:v>
+                  <c:v>0.79757800000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>107.42950399999999</c:v>
+                  <c:v>0.89619400000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>116.45775</c:v>
+                  <c:v>0.99653999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>125.50593600000001</c:v>
+                  <c:v>1.0165999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>134.09773000000001</c:v>
+                  <c:v>1.9921800000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>143.59235000000001</c:v>
+                  <c:v>2.9991400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -741,52 +672,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>64.364450000000005</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109.88923</c:v>
+                  <c:v>1.48568E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>129.6439</c:v>
+                  <c:v>2.7317399999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>135.57826</c:v>
+                  <c:v>1.42578</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>136.48705000000001</c:v>
+                  <c:v>3.37921</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>132.98442</c:v>
+                  <c:v>13.379799999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>126.99706999999999</c:v>
+                  <c:v>26.4255</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>119.08304</c:v>
+                  <c:v>36.149099999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>111.82526</c:v>
+                  <c:v>45.040199999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>105.837906</c:v>
+                  <c:v>52.824199999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>99.222350000000006</c:v>
+                  <c:v>59.777700000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>91.336380000000005</c:v>
+                  <c:v>64.791200000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85.334999999999994</c:v>
+                  <c:v>69.251099999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>78.077219999999997</c:v>
+                  <c:v>68.905299999999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>71.433610000000002</c:v>
+                  <c:v>107.75700000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>64.189864999999998</c:v>
+                  <c:v>132.02199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2565,17 +2496,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2586,210 +2517,619 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0.12218999999999999</v>
-      </c>
-      <c r="B2">
-        <v>201.81899999999999</v>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>197.297</v>
       </c>
       <c r="E2">
-        <v>9.1478859999999997</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>64.364450000000005</v>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7.9600897000000002</v>
-      </c>
-      <c r="B3">
-        <v>150.17026999999999</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4.9495499999999998E-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>162.184</v>
       </c>
       <c r="E3">
-        <v>17.805035</v>
+        <v>5.3633199999999999E-2</v>
       </c>
       <c r="F3">
-        <v>109.88923</v>
+        <v>1.48568E-2</v>
+      </c>
+      <c r="I3">
+        <v>6.3268900000000003E-2</v>
+      </c>
+      <c r="J3">
+        <v>0.110385</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>17.499040000000001</v>
-      </c>
-      <c r="B4">
-        <v>111.00869</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>9.7603599999999999E-2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>121.215</v>
       </c>
       <c r="E4">
-        <v>26.424519</v>
+        <v>9.8615900000000006E-2</v>
       </c>
       <c r="F4">
-        <v>129.6439</v>
+        <v>2.7317399999999999E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.105448</v>
+      </c>
+      <c r="J4">
+        <v>0.78335699999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>26.761690000000002</v>
-      </c>
-      <c r="B5">
-        <v>88.492249999999999</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.14979799999999999</v>
+      </c>
+      <c r="B5" s="1">
+        <v>99.166600000000003</v>
       </c>
       <c r="E5">
-        <v>35.263339999999999</v>
+        <v>0.147059</v>
       </c>
       <c r="F5">
-        <v>135.57826</v>
+        <v>1.42578</v>
+      </c>
+      <c r="I5">
+        <v>0.14762700000000001</v>
+      </c>
+      <c r="J5">
+        <v>1.5686899999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>35.514499999999998</v>
-      </c>
-      <c r="B6">
-        <v>69.915450000000007</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.19775400000000001</v>
+      </c>
+      <c r="B6" s="1">
+        <v>79.818799999999996</v>
       </c>
       <c r="E6">
-        <v>44.181919999999998</v>
+        <v>0.198962</v>
       </c>
       <c r="F6">
-        <v>136.48705000000001</v>
+        <v>3.37921</v>
+      </c>
+      <c r="I6">
+        <v>0.20386599999999999</v>
+      </c>
+      <c r="J6">
+        <v>4.0390199999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>54.506880000000002</v>
-      </c>
-      <c r="B7">
-        <v>50.293564000000003</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.29777199999999998</v>
+      </c>
+      <c r="B7" s="1">
+        <v>57.341299999999997</v>
       </c>
       <c r="E7">
-        <v>52.723860000000002</v>
+        <v>0.30103799999999997</v>
       </c>
       <c r="F7">
-        <v>132.98442</v>
+        <v>13.379799999999999</v>
+      </c>
+      <c r="I7">
+        <v>0.30228500000000003</v>
+      </c>
+      <c r="J7">
+        <v>10.8902</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>72.426950000000005</v>
-      </c>
-      <c r="B8">
-        <v>41.721465999999999</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.39771000000000001</v>
+      </c>
+      <c r="B8" s="1">
+        <v>46.125100000000003</v>
       </c>
       <c r="E8">
-        <v>62.198535999999997</v>
+        <v>0.39619399999999999</v>
       </c>
       <c r="F8">
-        <v>126.99706999999999</v>
+        <v>26.4255</v>
+      </c>
+      <c r="I8">
+        <v>0.40070299999999998</v>
+      </c>
+      <c r="J8">
+        <v>16.617799999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>90.751599999999996</v>
-      </c>
-      <c r="B9">
-        <v>35.550727999999999</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.49480299999999999</v>
+      </c>
+      <c r="B9" s="1">
+        <v>39.412100000000002</v>
       </c>
       <c r="E9">
-        <v>70.363839999999996</v>
+        <v>0.49826999999999999</v>
       </c>
       <c r="F9">
-        <v>119.08304</v>
+        <v>36.149099999999997</v>
+      </c>
+      <c r="I9">
+        <v>0.49912099999999998</v>
+      </c>
+      <c r="J9">
+        <v>21.109400000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>108.60589</v>
-      </c>
-      <c r="B10">
-        <v>30.941756999999999</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.59469700000000003</v>
+      </c>
+      <c r="B10" s="1">
+        <v>34.502099999999999</v>
       </c>
       <c r="E10">
-        <v>79.412025</v>
+        <v>0.59515600000000002</v>
       </c>
       <c r="F10">
-        <v>111.82526</v>
+        <v>45.040199999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.60456900000000002</v>
+      </c>
+      <c r="J10">
+        <v>22.454699999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>126.01612</v>
-      </c>
-      <c r="B11">
-        <v>26.3093</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.69459400000000004</v>
+      </c>
+      <c r="B11" s="1">
+        <v>29.1417</v>
       </c>
       <c r="E11">
-        <v>88.886700000000005</v>
+        <v>0.69550199999999995</v>
       </c>
       <c r="F11">
-        <v>105.837906</v>
+        <v>52.824199999999998</v>
+      </c>
+      <c r="I11">
+        <v>0.69595799999999997</v>
+      </c>
+      <c r="J11">
+        <v>23.912800000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>144.24867</v>
-      </c>
-      <c r="B12">
-        <v>25.686942999999999</v>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.79308199999999995</v>
+      </c>
+      <c r="B12" s="1">
+        <v>24.231100000000001</v>
       </c>
       <c r="E12">
-        <v>98.371346000000003</v>
+        <v>0.79757800000000001</v>
       </c>
       <c r="F12">
-        <v>99.222350000000006</v>
+        <v>59.777700000000003</v>
+      </c>
+      <c r="I12">
+        <v>0.80843600000000004</v>
+      </c>
+      <c r="J12">
+        <v>25.595099999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>162.93843000000001</v>
-      </c>
-      <c r="B13">
-        <v>24.295444</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.892953</v>
+      </c>
+      <c r="B13" s="1">
+        <v>22.474299999999999</v>
       </c>
       <c r="E13">
-        <v>107.42950399999999</v>
+        <v>0.89619400000000005</v>
       </c>
       <c r="F13">
-        <v>91.336380000000005</v>
+        <v>64.791200000000003</v>
+      </c>
+      <c r="I13">
+        <v>0.90685400000000005</v>
+      </c>
+      <c r="J13">
+        <v>26.715900000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.99423499999999998</v>
+      </c>
+      <c r="B14" s="1">
+        <v>20.267700000000001</v>
+      </c>
       <c r="E14">
-        <v>116.45775</v>
+        <v>0.99653999999999998</v>
       </c>
       <c r="F14">
-        <v>85.334999999999994</v>
+        <v>69.251099999999994</v>
+      </c>
+      <c r="I14">
+        <v>0.99824299999999999</v>
+      </c>
+      <c r="J14">
+        <v>26.7133</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>19.579899999999999</v>
+      </c>
       <c r="E15">
-        <v>125.50593600000001</v>
+        <v>1.0165999999999999</v>
       </c>
       <c r="F15">
-        <v>78.077219999999997</v>
+        <v>68.905299999999997</v>
+      </c>
+      <c r="I15">
+        <v>1.51142</v>
+      </c>
+      <c r="J15">
+        <v>22.766300000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.9886999999999999</v>
+      </c>
+      <c r="B16">
+        <v>11.676600000000001</v>
+      </c>
       <c r="E16">
-        <v>134.09773000000001</v>
+        <v>1.9921800000000001</v>
       </c>
       <c r="F16">
-        <v>71.433610000000002</v>
+        <v>107.75700000000001</v>
+      </c>
+      <c r="I16">
+        <v>2.0035099999999999</v>
+      </c>
+      <c r="J16">
+        <v>16.235700000000001</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2.9519799999999998</v>
+      </c>
+      <c r="B17">
+        <v>9.0782100000000003</v>
+      </c>
       <c r="E17">
-        <v>143.59235000000001</v>
+        <v>2.9991400000000001</v>
       </c>
       <c r="F17">
-        <v>64.189864999999998</v>
+        <v>132.02199999999999</v>
+      </c>
+      <c r="I17">
+        <v>2.52373</v>
+      </c>
+      <c r="J17">
+        <v>11.277200000000001</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>3</v>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.9463300000000001</v>
+      </c>
+      <c r="B18">
+        <v>6.9876199999999997</v>
+      </c>
+      <c r="E18">
+        <v>4.0712799999999998</v>
+      </c>
+      <c r="F18">
+        <v>138.16300000000001</v>
+      </c>
+      <c r="I18">
+        <v>3.02285</v>
+      </c>
+      <c r="J18">
+        <v>7.8924200000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4.9096000000000002</v>
+      </c>
+      <c r="B19">
+        <v>5.7436100000000003</v>
+      </c>
+      <c r="E19">
+        <v>5.0036300000000002</v>
+      </c>
+      <c r="F19">
+        <v>136.79499999999999</v>
+      </c>
+      <c r="I19">
+        <v>3.9929700000000001</v>
+      </c>
+      <c r="J19">
+        <v>3.9325800000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5.9350300000000002</v>
+      </c>
+      <c r="B20">
+        <v>5.0637800000000004</v>
+      </c>
+      <c r="E20">
+        <v>5.9701300000000002</v>
+      </c>
+      <c r="F20">
+        <v>133.65899999999999</v>
+      </c>
+      <c r="I20">
+        <v>4.0177300000000002</v>
+      </c>
+      <c r="J20">
+        <v>3.9042300000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6.9604499999999998</v>
+      </c>
+      <c r="B21">
+        <v>4.72255</v>
+      </c>
+      <c r="E21">
+        <v>6.9703200000000001</v>
+      </c>
+      <c r="F21">
+        <v>126.54300000000001</v>
+      </c>
+      <c r="I21">
+        <v>5.0709200000000001</v>
+      </c>
+      <c r="J21">
+        <v>2.3492999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7.9858799999999999</v>
+      </c>
+      <c r="B22">
+        <v>4.4377500000000003</v>
+      </c>
+      <c r="E22">
+        <v>7.9706099999999998</v>
+      </c>
+      <c r="F22">
+        <v>119.869</v>
+      </c>
+      <c r="I22">
+        <v>6.0461</v>
+      </c>
+      <c r="J22">
+        <v>1.6732400000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8.9491499999999995</v>
+      </c>
+      <c r="B23">
+        <v>4.2095500000000001</v>
+      </c>
+      <c r="E23">
+        <v>8.9360700000000008</v>
+      </c>
+      <c r="F23">
+        <v>111.87</v>
+      </c>
+      <c r="I23">
+        <v>7.02128</v>
+      </c>
+      <c r="J23">
+        <v>1.13239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9.9435000000000002</v>
+      </c>
+      <c r="B24">
+        <v>3.8683999999999998</v>
+      </c>
+      <c r="E24">
+        <v>9.9363499999999991</v>
+      </c>
+      <c r="F24">
+        <v>105.196</v>
+      </c>
+      <c r="I24">
+        <v>8.1134799999999991</v>
+      </c>
+      <c r="J24">
+        <v>0.82816900000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10.937900000000001</v>
+      </c>
+      <c r="B25">
+        <v>3.8094100000000002</v>
+      </c>
+      <c r="E25">
+        <v>10.936500000000001</v>
+      </c>
+      <c r="F25">
+        <v>98.080200000000005</v>
+      </c>
+      <c r="I25">
+        <v>9.1276600000000006</v>
+      </c>
+      <c r="J25">
+        <v>0.65915500000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>11.994400000000001</v>
+      </c>
+      <c r="B26">
+        <v>3.52454</v>
+      </c>
+      <c r="E26">
+        <v>11.936500000000001</v>
+      </c>
+      <c r="F26">
+        <v>90.080200000000005</v>
+      </c>
+      <c r="I26">
+        <v>10.1418</v>
+      </c>
+      <c r="J26">
+        <v>0.49014099999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12.926600000000001</v>
+      </c>
+      <c r="B27">
+        <v>3.4092799999999999</v>
+      </c>
+      <c r="E27">
+        <v>12.971299999999999</v>
+      </c>
+      <c r="F27">
+        <v>82.962599999999995</v>
+      </c>
+      <c r="I27">
+        <v>11.156000000000001</v>
+      </c>
+      <c r="J27">
+        <v>0.42253499999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>13.952</v>
+      </c>
+      <c r="B28">
+        <v>3.3502200000000002</v>
+      </c>
+      <c r="E28">
+        <v>13.9023</v>
+      </c>
+      <c r="F28">
+        <v>75.407600000000002</v>
+      </c>
+      <c r="I28">
+        <v>12.1312</v>
+      </c>
+      <c r="J28">
+        <v>0.37183100000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>14.9153</v>
+      </c>
+      <c r="B29">
+        <v>3.3477399999999999</v>
+      </c>
+      <c r="E29">
+        <v>14.867900000000001</v>
+      </c>
+      <c r="F29">
+        <v>68.293099999999995</v>
+      </c>
+      <c r="I29">
+        <v>13.106400000000001</v>
+      </c>
+      <c r="J29">
+        <v>0.30422500000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>15.9407</v>
+      </c>
+      <c r="B30">
+        <v>3.1758099999999998</v>
+      </c>
+      <c r="E30">
+        <v>15.868</v>
+      </c>
+      <c r="F30">
+        <v>60.735100000000003</v>
+      </c>
+      <c r="I30">
+        <v>14.159599999999999</v>
+      </c>
+      <c r="J30">
+        <v>0.253521</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>16.904</v>
+      </c>
+      <c r="B31">
+        <v>3.1169099999999998</v>
+      </c>
+      <c r="I31">
+        <v>15.1348</v>
+      </c>
+      <c r="J31">
+        <v>0.202817</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>17.898299999999999</v>
+      </c>
+      <c r="B32">
+        <v>3.34009</v>
+      </c>
+      <c r="I32">
+        <v>16.1099</v>
+      </c>
+      <c r="J32">
+        <v>0.202817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality for builder, added concrete data in cpp file
</commit_message>
<xml_diff>
--- a/Retina Project Beta/Topography Data.xlsx
+++ b/Retina Project Beta/Topography Data.xlsx
@@ -76,7 +76,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,7 +129,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Cone Densities</a:t>
+              <a:t>Cone</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -173,7 +173,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -196,17 +196,204 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!#REF!</c:f>
+              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9495499999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7603599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14979799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19775400000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29777199999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39771000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.49480299999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59469700000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69459400000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.79308199999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.892953</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99423499999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9886999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.9519799999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.9463300000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.9096000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9350300000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9604499999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.9858799999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.9491499999999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.9435000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.937900000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.994400000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.926600000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.952</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.9153</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15.9407</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16.904</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17.898299999999999</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!#REF!</c:f>
+              <c:f>Sheet1!$B$2:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>197.297</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>162.184</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>121.215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.166600000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79.818799999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.341299999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.125100000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.412100000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34.502099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.1417</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.231100000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.474299999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.267700000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.579899999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.676600000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.0782100000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.9876199999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.7436100000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.0637800000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.72255</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.4377500000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.2095500000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.8683999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.8094100000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.52454</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.4092799999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.3502200000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.3477399999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.1758099999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.1169099999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.34009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -214,7 +401,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-51A1-4A44-8A4B-C375E4EF887E}"/>
+              <c16:uniqueId val="{00000000-FAED-47A1-BBBF-DBE77EA3C8FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -226,11 +413,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1858030464"/>
-        <c:axId val="1861029520"/>
+        <c:axId val="377802096"/>
+        <c:axId val="381154624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1858030464"/>
+        <c:axId val="377802096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -250,61 +437,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Eccentricity (degrees)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -342,12 +474,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1861029520"/>
+        <c:crossAx val="381154624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1861029520"/>
+        <c:axId val="381154624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -367,61 +499,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Cones/mm2 (x1000)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -459,7 +536,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1858030464"/>
+        <c:crossAx val="377802096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -543,7 +620,488 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Rod Densities</a:t>
+              <a:t>Rod</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3633199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8615900000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.147059</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.198962</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30103799999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39619399999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.49826999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59515600000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69550199999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.79757800000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.89619400000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99653999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0165999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9921800000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.9991400000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.0712799999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.0036300000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9701300000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9703200000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.9706099999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.9360700000000008</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.9363499999999991</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.936500000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.936500000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.971299999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.9023</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.867900000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15.868</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.48568E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7317399999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.42578</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.37921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.379799999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.4255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.149099999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.040199999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.824199999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.777700000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.791200000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>69.251099999999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>68.905299999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>107.75700000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>132.02199999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>138.16300000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>136.79499999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>133.65899999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>126.54300000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>119.869</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>111.87</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>105.196</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>98.080200000000005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>90.080200000000005</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>82.962599999999995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>75.407600000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>68.293099999999995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>60.735100000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-52BC-466F-9ABE-75F3C792303E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="377816512"/>
+        <c:axId val="381135616"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="377816512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="381135616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="381135616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377816512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ganglion</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -610,114 +1168,204 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$17</c:f>
+              <c:f>Sheet1!$I$2:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3633199999999999E-2</c:v>
+                  <c:v>6.3268900000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.8615900000000006E-2</c:v>
+                  <c:v>0.105448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.147059</c:v>
+                  <c:v>0.14762700000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.198962</c:v>
+                  <c:v>0.20386599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30103799999999997</c:v>
+                  <c:v>0.30228500000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39619399999999999</c:v>
+                  <c:v>0.40070299999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.49826999999999999</c:v>
+                  <c:v>0.49912099999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.59515600000000002</c:v>
+                  <c:v>0.60456900000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.69550199999999995</c:v>
+                  <c:v>0.69595799999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.79757800000000001</c:v>
+                  <c:v>0.80843600000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.89619400000000005</c:v>
+                  <c:v>0.90685400000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.99653999999999998</c:v>
+                  <c:v>0.99824299999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0165999999999999</c:v>
+                  <c:v>1.51142</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9921800000000001</c:v>
+                  <c:v>2.0035099999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.9991400000000001</c:v>
+                  <c:v>2.52373</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.02285</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9929700000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0177300000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0709200000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.0461</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.02128</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.1134799999999991</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1276600000000006</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10.1418</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.156000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12.1312</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.106400000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.159599999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15.1348</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>16.1099</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$17</c:f>
+              <c:f>Sheet1!$J$2:$J$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.48568E-2</c:v>
+                  <c:v>0.110385</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7317399999999999E-2</c:v>
+                  <c:v>0.78335699999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.42578</c:v>
+                  <c:v>1.5686899999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.37921</c:v>
+                  <c:v>4.0390199999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.379799999999999</c:v>
+                  <c:v>10.8902</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.4255</c:v>
+                  <c:v>16.617799999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.149099999999997</c:v>
+                  <c:v>21.109400000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45.040199999999999</c:v>
+                  <c:v>22.454699999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.824199999999998</c:v>
+                  <c:v>23.912800000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>59.777700000000003</c:v>
+                  <c:v>25.595099999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64.791200000000003</c:v>
+                  <c:v>26.715900000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>69.251099999999994</c:v>
+                  <c:v>26.7133</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>68.905299999999997</c:v>
+                  <c:v>22.766300000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>107.75700000000001</c:v>
+                  <c:v>16.235700000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>132.02199999999999</c:v>
+                  <c:v>11.277200000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.8924200000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9325800000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.9042300000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.3492999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.6732400000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.13239</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.82816900000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.65915500000000005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.49014099999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.42253499999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.37183100000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.30422500000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.253521</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.202817</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.202817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,7 +1373,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-096D-4D41-9019-5019B2BCA2CE}"/>
+              <c16:uniqueId val="{00000000-009E-4ED3-A534-71CDCC64285D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -737,11 +1385,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1865650176"/>
-        <c:axId val="1743380240"/>
+        <c:axId val="375644496"/>
+        <c:axId val="373868112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1865650176"/>
+        <c:axId val="375644496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,61 +1409,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Eccentricity (degrees)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -853,77 +1446,31 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1743380240"/>
+        <c:crossAx val="373868112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1743380240"/>
+        <c:axId val="373868112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Rods/mm2</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (X1000)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
+        <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -961,7 +1508,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1865650176"/>
+        <c:crossAx val="375644496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1090,6 +1637,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2122,27 +2709,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79530B2A-604D-4CE0-9CD5-E1E6476651A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EE5549E-A9FC-4F24-A293-042965743F5F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2162,23 +3265,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9508A78-D5B8-4667-990D-2C877B09FC1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA5B746B-6D71-48D3-9D47-461188557C0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2191,6 +3294,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D706582-EC9D-44CC-B080-79C7FDB8C04E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2498,8 +3637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix for bug in rod generation
</commit_message>
<xml_diff>
--- a/Retina Project Beta/Topography Data.xlsx
+++ b/Retina Project Beta/Topography Data.xlsx
@@ -108,62 +108,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Cone</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -173,25 +118,39 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -427,9 +386,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -437,6 +397,73 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Eccentricity</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" baseline="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="0">
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -445,9 +472,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -461,14 +487,13 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -489,9 +514,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -499,6 +525,80 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Density (cells/mm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" baseline="30000">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" baseline="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="0">
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -507,9 +607,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -523,14 +622,13 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -554,11 +652,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -918,6 +1019,36 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -980,6 +1111,36 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1678,6 +1839,544 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2193,7 +2892,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2709,536 +3408,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3265,16 +3448,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3302,15 +3485,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3637,8 +3820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>